<commit_message>
stock and buffer page
</commit_message>
<xml_diff>
--- a/WRX_SAP INTERFACE/Flex_Data_structure.xlsx
+++ b/WRX_SAP INTERFACE/Flex_Data_structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flex\WRX_SAP INTERFACE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CD5186-010F-41E4-B146-A6E86C128875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BB5466-9539-48E0-BCB1-8BC97761ED31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12C5C8EF-92D1-47ED-8473-DFC0E0C05236}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="337">
   <si>
     <t>Menu Group</t>
   </si>
@@ -1042,6 +1042,12 @@
   </si>
   <si>
     <t>Vender</t>
+  </si>
+  <si>
+    <t>ICCKST</t>
+  </si>
+  <si>
+    <t>ตรวจสอบ Stock</t>
   </si>
 </sst>
 </file>
@@ -10434,10 +10440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB82F9EC-2777-44E0-A7BB-7F93552DDD25}">
-  <dimension ref="B3:P82"/>
+  <dimension ref="B3:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11099,37 +11105,30 @@
       </c>
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E33" s="34" t="s">
-        <v>285</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H33" s="4" t="s">
+      <c r="F33" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="H33" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I33" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
     </row>
     <row r="34" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E34" s="34" t="s">
         <v>285</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>1</v>
@@ -11138,42 +11137,44 @@
         <v>64</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E35" s="34" t="s">
         <v>285</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E36" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G36" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="O35" s="29"/>
-    </row>
-    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="F36" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>1</v>
@@ -11182,20 +11183,19 @@
         <v>64</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
+        <v>126</v>
+      </c>
+      <c r="O36" s="29"/>
     </row>
     <row r="37" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F37" s="5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>1</v>
@@ -11204,53 +11204,52 @@
         <v>64</v>
       </c>
       <c r="J37" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="O37" s="30"/>
+      <c r="P37" s="30"/>
+    </row>
+    <row r="38" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="K38" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="F38" s="32" t="s">
+    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="F39" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G38" s="32" t="s">
+      <c r="G39" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="H38" s="33" t="s">
+      <c r="H39" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I38" s="32" t="s">
+      <c r="I39" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="J38" s="32" t="s">
+      <c r="J39" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="K38" s="32" t="s">
+      <c r="K39" s="32" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E39" s="34" t="s">
-        <v>285</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="40" spans="5:16" x14ac:dyDescent="0.25">
@@ -11258,10 +11257,10 @@
         <v>285</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>1</v>
@@ -11270,10 +11269,10 @@
         <v>64</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.25">
@@ -11281,10 +11280,10 @@
         <v>285</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>1</v>
@@ -11293,10 +11292,10 @@
         <v>64</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="5:16" x14ac:dyDescent="0.25">
@@ -11304,10 +11303,10 @@
         <v>285</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>1</v>
@@ -11316,19 +11315,21 @@
         <v>64</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E43" s="34"/>
+      <c r="E43" s="34" t="s">
+        <v>285</v>
+      </c>
       <c r="F43" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>1</v>
@@ -11337,21 +11338,19 @@
         <v>64</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E44" s="34" t="s">
-        <v>285</v>
-      </c>
+      <c r="E44" s="34"/>
       <c r="F44" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="H44" s="6" t="s">
         <v>1</v>
@@ -11360,10 +11359,10 @@
         <v>64</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="5:16" x14ac:dyDescent="0.25">
@@ -11371,43 +11370,46 @@
         <v>285</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="46" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E46" s="34" t="s">
         <v>285</v>
       </c>
       <c r="F46" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="G46" s="5"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E47" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G46" s="5" t="s">
+      <c r="G47" s="5" t="s">
         <v>269</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="F47" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>270</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>1</v>
@@ -11416,7 +11418,7 @@
         <v>64</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>271</v>
+        <v>65</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>133</v>
@@ -11424,10 +11426,10 @@
     </row>
     <row r="48" spans="5:16" x14ac:dyDescent="0.25">
       <c r="F48" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>1</v>
@@ -11436,19 +11438,18 @@
         <v>64</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="L48" s="27"/>
-    </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F49" s="5" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>1</v>
@@ -11457,18 +11458,19 @@
         <v>64</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>304</v>
+        <v>274</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+      <c r="L49" s="27"/>
+    </row>
+    <row r="50" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F50" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>1</v>
@@ -11477,49 +11479,61 @@
         <v>64</v>
       </c>
       <c r="J50" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="51" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F51" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J51" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="K50" s="5" t="s">
+      <c r="K51" s="5" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="51" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F52" s="3" t="s">
+    <row r="52" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F53" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="H52" s="4" t="s">
+      <c r="H53" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I52" s="3" t="s">
+      <c r="I53" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="J52" s="3" t="s">
+      <c r="J53" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="K52" s="3" t="s">
+      <c r="K53" s="3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="53" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-    </row>
-    <row r="54" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="4"/>
@@ -11527,32 +11541,20 @@
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
     </row>
-    <row r="55" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F55" s="32" t="s">
+    <row r="55" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F56" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="G55" s="32" t="s">
+      <c r="G56" s="32" t="s">
         <v>94</v>
-      </c>
-      <c r="H55" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="I55" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="J55" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="K55" s="32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F56" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="G56" s="32" t="s">
-        <v>95</v>
       </c>
       <c r="H56" s="33" t="s">
         <v>5</v>
@@ -11561,38 +11563,38 @@
         <v>104</v>
       </c>
       <c r="J56" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="K56" s="32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F57" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G57" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="H57" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I57" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="J57" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="K56" s="32" t="s">
+      <c r="K57" s="32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F57" s="5" t="s">
+    <row r="58" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F58" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G57" s="5" t="s">
+      <c r="G58" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="K57" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F58" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>5</v>
@@ -11601,38 +11603,38 @@
         <v>103</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="59" spans="5:11" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F59" s="5" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="5:11" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F60" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>5</v>
@@ -11641,18 +11643,18 @@
         <v>96</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="61" spans="5:11" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F61" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>5</v>
@@ -11661,36 +11663,47 @@
         <v>96</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="62" spans="5:11" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="62" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F62" s="5" t="s">
-        <v>266</v>
+        <v>73</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>267</v>
+        <v>80</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-    </row>
-    <row r="63" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-    </row>
-    <row r="64" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E64" s="34"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="4"/>
+      <c r="I62" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F63" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+    </row>
+    <row r="64" spans="6:12" x14ac:dyDescent="0.25">
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
@@ -11706,32 +11719,20 @@
     </row>
     <row r="66" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E66" s="34"/>
-      <c r="F66" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I66" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="J66" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K66" s="5" t="s">
-        <v>136</v>
-      </c>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
     </row>
     <row r="67" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E67" s="34"/>
       <c r="F67" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>2</v>
@@ -11740,18 +11741,19 @@
         <v>63</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="68" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E68" s="34"/>
       <c r="F68" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>2</v>
@@ -11760,19 +11762,18 @@
         <v>63</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E69" s="34"/>
       <c r="F69" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>2</v>
@@ -11781,57 +11782,72 @@
         <v>63</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K69" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="70" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F70" s="27" t="s">
+      <c r="E70" s="34"/>
+      <c r="F70" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K70" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F71" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="G70" s="27" t="s">
+      <c r="G71" s="27" t="s">
         <v>231</v>
       </c>
-      <c r="H70" s="28" t="s">
+      <c r="H71" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="I70" s="27" t="s">
+      <c r="I71" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="J70" s="27" t="s">
+      <c r="J71" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="K70" s="27" t="s">
+      <c r="K71" s="27" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="71" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F71" s="5" t="s">
+    <row r="72" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F72" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="G71" s="5" t="s">
+      <c r="G72" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="H71" s="6" t="s">
+      <c r="H72" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I72" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="J71" s="5" t="s">
+      <c r="J72" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="K71" s="5" t="s">
+      <c r="K72" s="5" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="72" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F72" s="25"/>
-      <c r="G72" s="26"/>
-      <c r="H72" s="24"/>
-      <c r="I72" s="26"/>
     </row>
     <row r="73" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F73" s="25"/>
@@ -11846,30 +11862,25 @@
       <c r="I74" s="26"/>
     </row>
     <row r="75" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F75" s="38" t="s">
+      <c r="F75" s="25"/>
+      <c r="G75" s="26"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="26"/>
+    </row>
+    <row r="76" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F76" s="38" t="s">
         <v>282</v>
       </c>
-      <c r="G75" s="39"/>
-      <c r="H75" s="39"/>
-      <c r="I75" s="26"/>
-    </row>
-    <row r="76" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F76" s="25" t="s">
+      <c r="G76" s="39"/>
+      <c r="H76" s="39"/>
+      <c r="I76" s="26"/>
+    </row>
+    <row r="77" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F77" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G77" t="s">
         <v>230</v>
-      </c>
-      <c r="H76" s="24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="F77" t="s">
-        <v>227</v>
-      </c>
-      <c r="G77" t="s">
-        <v>214</v>
       </c>
       <c r="H77" s="24" t="s">
         <v>2</v>
@@ -11877,10 +11888,10 @@
     </row>
     <row r="78" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F78" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G78" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H78" s="24" t="s">
         <v>2</v>
@@ -11888,10 +11899,10 @@
     </row>
     <row r="79" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F79" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G79" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="H79" s="24" t="s">
         <v>2</v>
@@ -11899,10 +11910,10 @@
     </row>
     <row r="80" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G80" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H80" s="24" t="s">
         <v>2</v>
@@ -11910,36 +11921,47 @@
     </row>
     <row r="81" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
+        <v>226</v>
+      </c>
+      <c r="G81" t="s">
+        <v>224</v>
+      </c>
+      <c r="H81" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
         <v>260</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G82" t="s">
         <v>261</v>
       </c>
-      <c r="H81" s="24" t="s">
+      <c r="H82" s="24" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="82" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F82" s="3" t="s">
+    <row r="83" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F83" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="G82" s="3" t="s">
+      <c r="G83" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="H82" s="4" t="s">
+      <c r="H83" s="4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F5:J69">
-    <sortCondition ref="H5:H69"/>
-    <sortCondition ref="I5:I69"/>
-    <sortCondition ref="J5:J69"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F5:J70">
+    <sortCondition ref="H5:H70"/>
+    <sortCondition ref="I5:I70"/>
+    <sortCondition ref="J5:J70"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F76:H76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add feature adjust stock
</commit_message>
<xml_diff>
--- a/WRX_SAP INTERFACE/Flex_Data_structure.xlsx
+++ b/WRX_SAP INTERFACE/Flex_Data_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flex\WRX_SAP INTERFACE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179DE048-CFEC-4E51-9A49-3CEDA7EDF73B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E9FAE1-C4F6-49C1-A908-9CC101CE8B0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12C5C8EF-92D1-47ED-8473-DFC0E0C05236}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{12C5C8EF-92D1-47ED-8473-DFC0E0C05236}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="360">
   <si>
     <t>Menu Group</t>
   </si>
@@ -1101,6 +1101,24 @@
   </si>
   <si>
     <t>order_quotation, order_quotation_detail</t>
+  </si>
+  <si>
+    <t>RICSTB</t>
+  </si>
+  <si>
+    <t>รายงานสินค้าคงเหลือ</t>
+  </si>
+  <si>
+    <t>RSCSPD</t>
+  </si>
+  <si>
+    <t>รายงานยอดขาย แยกตามลูกค้า แสดงรายการสินค้า</t>
+  </si>
+  <si>
+    <t>RSCSBL</t>
+  </si>
+  <si>
+    <t>รายงานยอดขาย แยกตามลูกค้า แสดงยอดค้างรับ</t>
   </si>
 </sst>
 </file>
@@ -1358,7 +1376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1430,6 +1448,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1463,6 +1484,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="จุลภาค" xfId="1" builtinId="3"/>
@@ -10487,10 +10510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB82F9EC-2777-44E0-A7BB-7F93552DDD25}">
-  <dimension ref="B3:P82"/>
+  <dimension ref="B3:P95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="K65" sqref="K65"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10508,17 +10531,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="F3" s="36" t="s">
+      <c r="C3" s="36"/>
+      <c r="F3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -11991,94 +12014,184 @@
     </row>
     <row r="75" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E75" s="32"/>
-      <c r="F75" s="38" t="s">
-        <v>275</v>
-      </c>
-      <c r="G75" s="39"/>
-      <c r="H75" s="39"/>
-      <c r="I75" s="26"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="48"/>
+      <c r="H75" s="35"/>
+      <c r="I75" s="48"/>
     </row>
     <row r="76" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E76" s="32"/>
-      <c r="F76" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="G76" t="s">
-        <v>223</v>
-      </c>
-      <c r="H76" s="24" t="s">
-        <v>2</v>
-      </c>
+      <c r="F76" s="47"/>
+      <c r="G76" s="48"/>
+      <c r="H76" s="35"/>
+      <c r="I76" s="48"/>
     </row>
     <row r="77" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E77" s="32"/>
-      <c r="F77" t="s">
-        <v>220</v>
-      </c>
-      <c r="G77" t="s">
-        <v>207</v>
-      </c>
-      <c r="H77" s="24" t="s">
-        <v>2</v>
-      </c>
+      <c r="F77" s="47"/>
+      <c r="G77" s="48"/>
+      <c r="H77" s="35"/>
+      <c r="I77" s="48"/>
     </row>
     <row r="78" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E78" s="32"/>
-      <c r="F78" t="s">
-        <v>221</v>
-      </c>
-      <c r="G78" t="s">
-        <v>208</v>
-      </c>
-      <c r="H78" s="24" t="s">
-        <v>2</v>
-      </c>
+      <c r="F78" s="47" t="s">
+        <v>354</v>
+      </c>
+      <c r="G78" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="H78" s="35"/>
+      <c r="I78" s="48"/>
     </row>
     <row r="79" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E79" s="32"/>
-      <c r="F79" t="s">
-        <v>218</v>
-      </c>
-      <c r="G79" t="s">
-        <v>216</v>
-      </c>
-      <c r="H79" s="24" t="s">
-        <v>2</v>
-      </c>
+      <c r="F79" s="47" t="s">
+        <v>356</v>
+      </c>
+      <c r="G79" s="48" t="s">
+        <v>357</v>
+      </c>
+      <c r="H79" s="35"/>
+      <c r="I79" s="48"/>
     </row>
     <row r="80" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E80" s="32"/>
-      <c r="F80" t="s">
+      <c r="F80" s="47" t="s">
+        <v>358</v>
+      </c>
+      <c r="G80" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="H80" s="35"/>
+      <c r="I80" s="48"/>
+    </row>
+    <row r="81" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E81" s="32"/>
+      <c r="F81" s="47"/>
+      <c r="G81" s="48"/>
+      <c r="H81" s="35"/>
+      <c r="I81" s="48"/>
+    </row>
+    <row r="82" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E82" s="32"/>
+      <c r="F82" s="47"/>
+      <c r="G82" s="48"/>
+      <c r="H82" s="35"/>
+      <c r="I82" s="48"/>
+    </row>
+    <row r="83" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F83" s="47"/>
+      <c r="G83" s="48"/>
+      <c r="H83" s="35"/>
+      <c r="I83" s="48"/>
+    </row>
+    <row r="84" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F84" s="47"/>
+      <c r="G84" s="48"/>
+      <c r="H84" s="35"/>
+      <c r="I84" s="48"/>
+    </row>
+    <row r="85" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F85" s="47"/>
+      <c r="G85" s="48"/>
+      <c r="H85" s="35"/>
+      <c r="I85" s="48"/>
+    </row>
+    <row r="86" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F86" s="47"/>
+      <c r="G86" s="48"/>
+      <c r="H86" s="35"/>
+      <c r="I86" s="48"/>
+    </row>
+    <row r="87" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F87" s="47"/>
+      <c r="G87" s="48"/>
+      <c r="H87" s="35"/>
+      <c r="I87" s="48"/>
+    </row>
+    <row r="88" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F88" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="G88" s="40"/>
+      <c r="H88" s="40"/>
+      <c r="I88" s="26"/>
+    </row>
+    <row r="89" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F89" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="G89" t="s">
+        <v>223</v>
+      </c>
+      <c r="H89" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
+        <v>220</v>
+      </c>
+      <c r="G90" t="s">
+        <v>207</v>
+      </c>
+      <c r="H90" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>221</v>
+      </c>
+      <c r="G91" t="s">
+        <v>208</v>
+      </c>
+      <c r="H91" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>218</v>
+      </c>
+      <c r="G92" t="s">
+        <v>216</v>
+      </c>
+      <c r="H92" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
         <v>219</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G93" t="s">
         <v>217</v>
       </c>
-      <c r="H80" s="24" t="s">
+      <c r="H93" s="24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E81" s="32"/>
-      <c r="F81" t="s">
+    <row r="94" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
         <v>253</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G94" t="s">
         <v>254</v>
       </c>
-      <c r="H81" s="24" t="s">
+      <c r="H94" s="24" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E82" s="32"/>
-      <c r="F82" s="3" t="s">
+    <row r="95" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F95" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="G82" s="3" t="s">
+      <c r="G95" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="H82" s="4" t="s">
+      <c r="H95" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -12091,7 +12204,7 @@
   <mergeCells count="3">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F88:H88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12114,10 +12227,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="41" t="s">
         <v>237</v>
       </c>
-      <c r="K3" s="40"/>
+      <c r="K3" s="41"/>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
@@ -12281,10 +12394,10 @@
       <c r="K21" s="31"/>
     </row>
     <row r="22" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J22" s="40" t="s">
+      <c r="J22" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="K22" s="40"/>
+      <c r="K22" s="41"/>
     </row>
     <row r="23" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
@@ -12429,13 +12542,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -12455,7 +12568,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="44" t="s">
         <v>168</v>
       </c>
       <c r="C6" s="15"/>
@@ -12464,28 +12577,28 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="44"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="15"/>
       <c r="D7" s="7"/>
       <c r="E7" s="15"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="44"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="15"/>
       <c r="D8" s="7"/>
       <c r="E8" s="15"/>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="15"/>
       <c r="D9" s="7"/>
       <c r="E9" s="15"/>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="15"/>
       <c r="D10" s="7"/>
       <c r="E10" s="15"/>
@@ -12499,7 +12612,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="42" t="s">
         <v>169</v>
       </c>
       <c r="C12" s="15"/>
@@ -12508,21 +12621,21 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="15"/>
       <c r="D13" s="7"/>
       <c r="E13" s="15"/>
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="15"/>
       <c r="D14" s="7"/>
       <c r="E14" s="15"/>
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="15"/>
       <c r="D15" s="7"/>
       <c r="E15" s="15"/>
@@ -12536,7 +12649,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="42" t="s">
         <v>170</v>
       </c>
       <c r="C17" s="15"/>
@@ -12545,21 +12658,21 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="41"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="15"/>
       <c r="D18" s="7"/>
       <c r="E18" s="15"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="15"/>
       <c r="D19" s="7"/>
       <c r="E19" s="15"/>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="41"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="15"/>
       <c r="D20" s="7"/>
       <c r="E20" s="15"/>
@@ -12573,7 +12686,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="42" t="s">
         <v>171</v>
       </c>
       <c r="C22" s="15"/>
@@ -12582,14 +12695,14 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="41"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="15"/>
       <c r="D23" s="7"/>
       <c r="E23" s="15"/>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="41"/>
+      <c r="B24" s="42"/>
       <c r="C24" s="15"/>
       <c r="D24" s="7"/>
       <c r="E24" s="15"/>
@@ -12603,7 +12716,7 @@
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="42" t="s">
         <v>172</v>
       </c>
       <c r="C26" s="15"/>
@@ -12612,14 +12725,14 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="41"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="15"/>
       <c r="D27" s="7"/>
       <c r="E27" s="15"/>
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="41"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="15"/>
       <c r="D28" s="7"/>
       <c r="E28" s="15"/>
@@ -12633,7 +12746,7 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="42" t="s">
         <v>173</v>
       </c>
       <c r="C30" s="15"/>
@@ -12642,7 +12755,7 @@
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="41"/>
+      <c r="B31" s="42"/>
       <c r="C31" s="15"/>
       <c r="D31" s="7"/>
       <c r="E31" s="15"/>
@@ -12708,13 +12821,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -12734,7 +12847,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="46" t="s">
         <v>176</v>
       </c>
       <c r="C6" s="15"/>
@@ -12743,21 +12856,21 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="15"/>
       <c r="D7" s="7"/>
       <c r="E7" s="15"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="41"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="15"/>
       <c r="D8" s="7"/>
       <c r="E8" s="15"/>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="15"/>
       <c r="D9" s="7"/>
       <c r="E9" s="15"/>
@@ -12812,7 +12925,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="42" t="s">
         <v>180</v>
       </c>
       <c r="C16" s="15"/>
@@ -12821,7 +12934,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="41"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="15"/>
       <c r="D17" s="7"/>
       <c r="E17" s="15"/>
@@ -12835,7 +12948,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="42" t="s">
         <v>181</v>
       </c>
       <c r="C19" s="15"/>
@@ -12844,7 +12957,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="41"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="15"/>
       <c r="D20" s="7"/>
       <c r="E20" s="15"/>
@@ -12890,7 +13003,7 @@
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="42" t="s">
         <v>184</v>
       </c>
       <c r="C26" s="15"/>
@@ -12899,7 +13012,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="41"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="15"/>
       <c r="D27" s="7"/>
       <c r="E27" s="15"/>
@@ -12913,7 +13026,7 @@
       <c r="F28" s="8"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="42" t="s">
         <v>185</v>
       </c>
       <c r="C29" s="15"/>
@@ -12922,7 +13035,7 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="41"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="15"/>
       <c r="D30" s="7"/>
       <c r="E30" s="15"/>
@@ -12936,7 +13049,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="42" t="s">
         <v>186</v>
       </c>
       <c r="C32" s="15"/>
@@ -12945,7 +13058,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="41"/>
+      <c r="B33" s="42"/>
       <c r="C33" s="15"/>
       <c r="D33" s="7"/>
       <c r="E33" s="15"/>
@@ -12959,7 +13072,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="42" t="s">
         <v>187</v>
       </c>
       <c r="C35" s="15"/>
@@ -12968,14 +13081,14 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="41"/>
+      <c r="B36" s="42"/>
       <c r="C36" s="15"/>
       <c r="D36" s="7"/>
       <c r="E36" s="15"/>
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="41"/>
+      <c r="B37" s="42"/>
       <c r="C37" s="15"/>
       <c r="D37" s="7"/>
       <c r="E37" s="15"/>
@@ -13099,14 +13212,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -13129,7 +13242,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="46" t="s">
         <v>189</v>
       </c>
       <c r="C6" s="19"/>
@@ -13139,7 +13252,7 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="19"/>
       <c r="D7" s="15"/>
       <c r="E7" s="7"/>
@@ -13147,7 +13260,7 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="41"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="19"/>
       <c r="D8" s="15"/>
       <c r="E8" s="7"/>
@@ -13163,7 +13276,7 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="42" t="s">
         <v>188</v>
       </c>
       <c r="C10" s="19"/>
@@ -13173,7 +13286,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="20"/>
       <c r="D11" s="15"/>
       <c r="E11" s="7"/>
@@ -13189,7 +13302,7 @@
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="42" t="s">
         <v>190</v>
       </c>
       <c r="C13" s="20"/>
@@ -13199,7 +13312,7 @@
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="20"/>
       <c r="D14" s="15"/>
       <c r="E14" s="7"/>
@@ -13207,7 +13320,7 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="20"/>
       <c r="D15" s="15"/>
       <c r="E15" s="7"/>
@@ -13223,7 +13336,7 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="42" t="s">
         <v>171</v>
       </c>
       <c r="C17" s="20"/>
@@ -13233,7 +13346,7 @@
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="41"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="20"/>
       <c r="D18" s="15"/>
       <c r="E18" s="7"/>
@@ -13241,7 +13354,7 @@
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="20"/>
       <c r="D19" s="15"/>
       <c r="E19" s="7"/>
@@ -13249,7 +13362,7 @@
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="42" t="s">
         <v>172</v>
       </c>
       <c r="C20" s="20"/>
@@ -13259,7 +13372,7 @@
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="41"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="20"/>
       <c r="D21" s="15"/>
       <c r="E21" s="7"/>
@@ -13275,7 +13388,7 @@
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>173</v>
       </c>
       <c r="C23" s="20"/>
@@ -13285,7 +13398,7 @@
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="41"/>
+      <c r="B24" s="42"/>
       <c r="C24" s="20"/>
       <c r="D24" s="15"/>
       <c r="E24" s="7"/>
@@ -13412,13 +13525,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -13694,13 +13807,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">

</xml_diff>

<commit_message>
fixed multi color code
</commit_message>
<xml_diff>
--- a/WRX_SAP INTERFACE/Flex_Data_structure.xlsx
+++ b/WRX_SAP INTERFACE/Flex_Data_structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flex\WRX_SAP INTERFACE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E9FAE1-C4F6-49C1-A908-9CC101CE8B0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75890E97-17EE-4E70-A54B-D74AAEFFFFCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{12C5C8EF-92D1-47ED-8473-DFC0E0C05236}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="362">
   <si>
     <t>Menu Group</t>
   </si>
@@ -1119,6 +1119,12 @@
   </si>
   <si>
     <t>รายงานยอดขาย แยกตามลูกค้า แสดงยอดค้างรับ</t>
+  </si>
+  <si>
+    <t>RICSBZ</t>
+  </si>
+  <si>
+    <t>รายงานสินค้าคงเหลือ แยกตามโซน</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1451,6 +1457,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1484,8 +1495,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="จุลภาค" xfId="1" builtinId="3"/>
@@ -10510,10 +10519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB82F9EC-2777-44E0-A7BB-7F93552DDD25}">
-  <dimension ref="B3:P95"/>
+  <dimension ref="B3:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="K83" sqref="K83"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10522,6 +10531,7 @@
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
     <col min="11" max="11" width="44" customWidth="1"/>
@@ -10531,17 +10541,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="39"/>
+      <c r="F3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -12014,127 +12024,135 @@
     </row>
     <row r="75" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E75" s="32"/>
-      <c r="F75" s="47"/>
-      <c r="G75" s="48"/>
+      <c r="F75" s="37"/>
+      <c r="G75" s="38"/>
       <c r="H75" s="35"/>
-      <c r="I75" s="48"/>
+      <c r="I75" s="38"/>
     </row>
     <row r="76" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E76" s="32"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="48"/>
+      <c r="F76" s="37"/>
+      <c r="G76" s="38"/>
       <c r="H76" s="35"/>
-      <c r="I76" s="48"/>
+      <c r="I76" s="38"/>
     </row>
     <row r="77" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E77" s="32"/>
-      <c r="F77" s="47"/>
-      <c r="G77" s="48"/>
+      <c r="F77" s="37"/>
+      <c r="G77" s="38"/>
       <c r="H77" s="35"/>
-      <c r="I77" s="48"/>
+      <c r="I77" s="38"/>
     </row>
     <row r="78" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E78" s="32"/>
-      <c r="F78" s="47" t="s">
+      <c r="F78" s="37" t="s">
         <v>354</v>
       </c>
-      <c r="G78" s="48" t="s">
+      <c r="G78" s="38" t="s">
         <v>355</v>
       </c>
-      <c r="H78" s="35"/>
-      <c r="I78" s="48"/>
+      <c r="H78" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="I78" s="38"/>
     </row>
     <row r="79" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E79" s="32"/>
-      <c r="F79" s="47" t="s">
-        <v>356</v>
-      </c>
-      <c r="G79" s="48" t="s">
-        <v>357</v>
-      </c>
-      <c r="H79" s="35"/>
-      <c r="I79" s="48"/>
+      <c r="F79" s="37" t="s">
+        <v>360</v>
+      </c>
+      <c r="G79" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="H79" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="I79" s="38"/>
     </row>
     <row r="80" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E80" s="32"/>
-      <c r="F80" s="47" t="s">
-        <v>358</v>
-      </c>
-      <c r="G80" s="48" t="s">
-        <v>359</v>
-      </c>
-      <c r="H80" s="35"/>
-      <c r="I80" s="48"/>
+      <c r="F80" s="37" t="s">
+        <v>356</v>
+      </c>
+      <c r="G80" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="H80" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="I80" s="38"/>
     </row>
     <row r="81" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E81" s="32"/>
-      <c r="F81" s="47"/>
-      <c r="G81" s="48"/>
-      <c r="H81" s="35"/>
-      <c r="I81" s="48"/>
+      <c r="F81" s="37" t="s">
+        <v>358</v>
+      </c>
+      <c r="G81" s="38" t="s">
+        <v>359</v>
+      </c>
+      <c r="H81" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="I81" s="38"/>
     </row>
     <row r="82" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E82" s="32"/>
-      <c r="F82" s="47"/>
-      <c r="G82" s="48"/>
+      <c r="F82" s="37"/>
+      <c r="G82" s="38"/>
       <c r="H82" s="35"/>
-      <c r="I82" s="48"/>
+      <c r="I82" s="38"/>
     </row>
     <row r="83" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F83" s="47"/>
-      <c r="G83" s="48"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="38"/>
       <c r="H83" s="35"/>
-      <c r="I83" s="48"/>
+      <c r="I83" s="38"/>
     </row>
     <row r="84" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F84" s="47"/>
-      <c r="G84" s="48"/>
+      <c r="F84" s="37"/>
+      <c r="G84" s="38"/>
       <c r="H84" s="35"/>
-      <c r="I84" s="48"/>
+      <c r="I84" s="38"/>
     </row>
     <row r="85" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F85" s="47"/>
-      <c r="G85" s="48"/>
+      <c r="F85" s="37"/>
+      <c r="G85" s="38"/>
       <c r="H85" s="35"/>
-      <c r="I85" s="48"/>
+      <c r="I85" s="38"/>
     </row>
     <row r="86" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F86" s="47"/>
-      <c r="G86" s="48"/>
+      <c r="F86" s="37"/>
+      <c r="G86" s="38"/>
       <c r="H86" s="35"/>
-      <c r="I86" s="48"/>
+      <c r="I86" s="38"/>
     </row>
     <row r="87" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F87" s="47"/>
-      <c r="G87" s="48"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="38"/>
       <c r="H87" s="35"/>
-      <c r="I87" s="48"/>
+      <c r="I87" s="38"/>
     </row>
     <row r="88" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F88" s="39" t="s">
+      <c r="F88" s="37"/>
+      <c r="G88" s="38"/>
+      <c r="H88" s="35"/>
+      <c r="I88" s="38"/>
+    </row>
+    <row r="89" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F89" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="G88" s="40"/>
-      <c r="H88" s="40"/>
-      <c r="I88" s="26"/>
-    </row>
-    <row r="89" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F89" s="25" t="s">
+      <c r="G89" s="43"/>
+      <c r="H89" s="43"/>
+      <c r="I89" s="26"/>
+    </row>
+    <row r="90" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F90" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G90" t="s">
         <v>223</v>
-      </c>
-      <c r="H89" s="24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F90" t="s">
-        <v>220</v>
-      </c>
-      <c r="G90" t="s">
-        <v>207</v>
       </c>
       <c r="H90" s="24" t="s">
         <v>2</v>
@@ -12142,10 +12160,10 @@
     </row>
     <row r="91" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F91" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G91" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H91" s="24" t="s">
         <v>2</v>
@@ -12153,10 +12171,10 @@
     </row>
     <row r="92" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F92" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G92" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H92" s="24" t="s">
         <v>2</v>
@@ -12164,10 +12182,10 @@
     </row>
     <row r="93" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F93" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H93" s="24" t="s">
         <v>2</v>
@@ -12175,23 +12193,34 @@
     </row>
     <row r="94" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F94" t="s">
+        <v>219</v>
+      </c>
+      <c r="G94" t="s">
+        <v>217</v>
+      </c>
+      <c r="H94" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
         <v>253</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G95" t="s">
         <v>254</v>
       </c>
-      <c r="H94" s="24" t="s">
+      <c r="H95" s="24" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F95" s="3" t="s">
+    <row r="96" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="F96" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="G95" s="3" t="s">
+      <c r="G96" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="H95" s="4" t="s">
+      <c r="H96" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -12204,7 +12233,7 @@
   <mergeCells count="3">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12215,7 +12244,7 @@
   <dimension ref="D3:K48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12227,10 +12256,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="K3" s="41"/>
+      <c r="K3" s="44"/>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
@@ -12394,10 +12423,10 @@
       <c r="K21" s="31"/>
     </row>
     <row r="22" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J22" s="41" t="s">
+      <c r="J22" s="44" t="s">
         <v>250</v>
       </c>
-      <c r="K22" s="41"/>
+      <c r="K22" s="44"/>
     </row>
     <row r="23" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
@@ -12530,7 +12559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13CBD5A-029C-499C-BF3D-7CDEF2F5D3FC}">
   <dimension ref="B4:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -12542,13 +12571,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -12568,7 +12597,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="47" t="s">
         <v>168</v>
       </c>
       <c r="C6" s="15"/>
@@ -12577,28 +12606,28 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="15"/>
       <c r="D7" s="7"/>
       <c r="E7" s="15"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="45"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="15"/>
       <c r="D8" s="7"/>
       <c r="E8" s="15"/>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="45"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="15"/>
       <c r="D9" s="7"/>
       <c r="E9" s="15"/>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="15"/>
       <c r="D10" s="7"/>
       <c r="E10" s="15"/>
@@ -12612,7 +12641,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="45" t="s">
         <v>169</v>
       </c>
       <c r="C12" s="15"/>
@@ -12621,21 +12650,21 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="42"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="15"/>
       <c r="D13" s="7"/>
       <c r="E13" s="15"/>
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="42"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="15"/>
       <c r="D14" s="7"/>
       <c r="E14" s="15"/>
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="15"/>
       <c r="D15" s="7"/>
       <c r="E15" s="15"/>
@@ -12649,7 +12678,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="45" t="s">
         <v>170</v>
       </c>
       <c r="C17" s="15"/>
@@ -12658,21 +12687,21 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="42"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="15"/>
       <c r="D18" s="7"/>
       <c r="E18" s="15"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="42"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="15"/>
       <c r="D19" s="7"/>
       <c r="E19" s="15"/>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="42"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="15"/>
       <c r="D20" s="7"/>
       <c r="E20" s="15"/>
@@ -12686,7 +12715,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="45" t="s">
         <v>171</v>
       </c>
       <c r="C22" s="15"/>
@@ -12695,14 +12724,14 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="42"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="15"/>
       <c r="D23" s="7"/>
       <c r="E23" s="15"/>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="42"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="15"/>
       <c r="D24" s="7"/>
       <c r="E24" s="15"/>
@@ -12716,7 +12745,7 @@
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="45" t="s">
         <v>172</v>
       </c>
       <c r="C26" s="15"/>
@@ -12725,14 +12754,14 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="42"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="15"/>
       <c r="D27" s="7"/>
       <c r="E27" s="15"/>
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="42"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="15"/>
       <c r="D28" s="7"/>
       <c r="E28" s="15"/>
@@ -12746,7 +12775,7 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="45" t="s">
         <v>173</v>
       </c>
       <c r="C30" s="15"/>
@@ -12755,7 +12784,7 @@
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="42"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="15"/>
       <c r="D31" s="7"/>
       <c r="E31" s="15"/>
@@ -12821,13 +12850,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -12847,7 +12876,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="49" t="s">
         <v>176</v>
       </c>
       <c r="C6" s="15"/>
@@ -12856,21 +12885,21 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="42"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="15"/>
       <c r="D7" s="7"/>
       <c r="E7" s="15"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="42"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="15"/>
       <c r="D8" s="7"/>
       <c r="E8" s="15"/>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="15"/>
       <c r="D9" s="7"/>
       <c r="E9" s="15"/>
@@ -12925,7 +12954,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="45" t="s">
         <v>180</v>
       </c>
       <c r="C16" s="15"/>
@@ -12934,7 +12963,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="42"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="15"/>
       <c r="D17" s="7"/>
       <c r="E17" s="15"/>
@@ -12948,7 +12977,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="45" t="s">
         <v>181</v>
       </c>
       <c r="C19" s="15"/>
@@ -12957,7 +12986,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="42"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="15"/>
       <c r="D20" s="7"/>
       <c r="E20" s="15"/>
@@ -13003,7 +13032,7 @@
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="45" t="s">
         <v>184</v>
       </c>
       <c r="C26" s="15"/>
@@ -13012,7 +13041,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="42"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="15"/>
       <c r="D27" s="7"/>
       <c r="E27" s="15"/>
@@ -13026,7 +13055,7 @@
       <c r="F28" s="8"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="45" t="s">
         <v>185</v>
       </c>
       <c r="C29" s="15"/>
@@ -13035,7 +13064,7 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="42"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="15"/>
       <c r="D30" s="7"/>
       <c r="E30" s="15"/>
@@ -13049,7 +13078,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="45" t="s">
         <v>186</v>
       </c>
       <c r="C32" s="15"/>
@@ -13058,7 +13087,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="42"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="15"/>
       <c r="D33" s="7"/>
       <c r="E33" s="15"/>
@@ -13072,7 +13101,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="45" t="s">
         <v>187</v>
       </c>
       <c r="C35" s="15"/>
@@ -13081,14 +13110,14 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="42"/>
+      <c r="B36" s="45"/>
       <c r="C36" s="15"/>
       <c r="D36" s="7"/>
       <c r="E36" s="15"/>
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="42"/>
+      <c r="B37" s="45"/>
       <c r="C37" s="15"/>
       <c r="D37" s="7"/>
       <c r="E37" s="15"/>
@@ -13199,7 +13228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE1C7F8-FF7A-4945-AD07-E9A5C590B338}">
   <dimension ref="B4:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -13212,14 +13241,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="46" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
     </row>
     <row r="5" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -13242,7 +13271,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="49" t="s">
         <v>189</v>
       </c>
       <c r="C6" s="19"/>
@@ -13252,7 +13281,7 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="42"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="19"/>
       <c r="D7" s="15"/>
       <c r="E7" s="7"/>
@@ -13260,7 +13289,7 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="42"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="19"/>
       <c r="D8" s="15"/>
       <c r="E8" s="7"/>
@@ -13276,7 +13305,7 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="45" t="s">
         <v>188</v>
       </c>
       <c r="C10" s="19"/>
@@ -13286,7 +13315,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="42"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="20"/>
       <c r="D11" s="15"/>
       <c r="E11" s="7"/>
@@ -13302,7 +13331,7 @@
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="45" t="s">
         <v>190</v>
       </c>
       <c r="C13" s="20"/>
@@ -13312,7 +13341,7 @@
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="42"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="20"/>
       <c r="D14" s="15"/>
       <c r="E14" s="7"/>
@@ -13320,7 +13349,7 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="20"/>
       <c r="D15" s="15"/>
       <c r="E15" s="7"/>
@@ -13336,7 +13365,7 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="45" t="s">
         <v>171</v>
       </c>
       <c r="C17" s="20"/>
@@ -13346,7 +13375,7 @@
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="42"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="20"/>
       <c r="D18" s="15"/>
       <c r="E18" s="7"/>
@@ -13354,7 +13383,7 @@
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="42"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="20"/>
       <c r="D19" s="15"/>
       <c r="E19" s="7"/>
@@ -13362,7 +13391,7 @@
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="45" t="s">
         <v>172</v>
       </c>
       <c r="C20" s="20"/>
@@ -13372,7 +13401,7 @@
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="42"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="20"/>
       <c r="D21" s="15"/>
       <c r="E21" s="7"/>
@@ -13388,7 +13417,7 @@
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="45" t="s">
         <v>173</v>
       </c>
       <c r="C23" s="20"/>
@@ -13398,7 +13427,7 @@
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="42"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="20"/>
       <c r="D24" s="15"/>
       <c r="E24" s="7"/>
@@ -13525,13 +13554,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
@@ -13795,7 +13824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327F71EA-3100-4F7C-95CD-CE4AC02F2294}">
   <dimension ref="B4:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -13807,13 +13836,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">

</xml_diff>